<commit_message>
fills PSD with created curves
</commit_message>
<xml_diff>
--- a/GPI Export to Curve PSD/SP Scripts/SPE Added Minimum Speed Curves.xlsx
+++ b/GPI Export to Curve PSD/SP Scripts/SPE Added Minimum Speed Curves.xlsx
@@ -1,62 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 1100S500-1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 150S100-2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 150S100-3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 150S100-5" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 150S250-10" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 150S250-12" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 150S250-7" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 150S400-15" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 150S400-20" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 150S500-25" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 230S100-2" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 230S250-4" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 230S250-6" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 230S250-7" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 230S400-10" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 230S400-12" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 230S500-15" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 300S100-1" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 300S100-2" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 300S250-4" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 300S250-6" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 300S400-10" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 300S400-8" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 300S500-12" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 300S500-13" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 385S100-1" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 385S250-2" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 385S250-3" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 385S400-4" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 385S400-5" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 385S500-6" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 475S250-1" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 475S250-2" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 475S400-3" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 475S400-4" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 475S500-5" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 625S250-1" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 625S500-2" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 800S400-1" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 85S100-2" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 85S100-4" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 85S100-6" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 85S100-8" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 85S250-10" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 85S250-12" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 85S250-16" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 85S250-20" sheetId="47" state="visible" r:id="rId47"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 85S400-24" sheetId="48" state="visible" r:id="rId48"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 85S400-28" sheetId="49" state="visible" r:id="rId49"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPE 85S500-36" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="SPE 1100S500-1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="SPE 150S100-2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="SPE 150S100-3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="SPE 150S100-5" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="SPE 150S250-10" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="SPE 150S250-12" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="SPE 150S250-7" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="SPE 150S400-15" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="SPE 150S400-20" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="SPE 150S500-25" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="SPE 230S100-2" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="SPE 230S250-4" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="SPE 230S250-6" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="SPE 230S250-7" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="SPE 230S400-10" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="SPE 230S400-12" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="SPE 230S500-15" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="SPE 300S100-1" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="SPE 300S100-2" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="SPE 300S250-4" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="SPE 300S250-6" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="SPE 300S400-10" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="SPE 300S400-8" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="SPE 300S500-12" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="SPE 300S500-13" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="SPE 385S100-1" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="SPE 385S250-2" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="SPE 385S250-3" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="SPE 385S400-4" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="SPE 385S400-5" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="SPE 385S500-6" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="SPE 475S250-1" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="SPE 475S250-2" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="SPE 475S400-3" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="SPE 475S400-4" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="SPE 475S500-5" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="SPE 625S250-1" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="SPE 625S500-2" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="SPE 800S400-1" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="SPE 85S100-2" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="SPE 85S100-4" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="SPE 85S100-6" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="SPE 85S100-8" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="SPE 85S250-10" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="SPE 85S250-12" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="SPE 85S250-16" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="SPE 85S250-20" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="SPE 85S400-24" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="SPE 85S400-28" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="SPE 85S500-36" sheetId="50" state="visible" r:id="rId50"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>